<commit_message>
refactor property part for create project by xls;
</commit_message>
<xml_diff>
--- a/app/res/xls/properties.xlsx
+++ b/app/res/xls/properties.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表 1" sheetId="1" r:id="rId4"/>
+    <sheet name="property" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -45,7 +45,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -57,9 +57,14 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="12"/>
@@ -67,12 +72,12 @@
       <name val="宋体"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b val="1"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -194,34 +199,34 @@
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1475,24 +1480,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozenSplit"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.05469" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.05469" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.05469" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.05469" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.05469" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.05469" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.05469" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.05469" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.05469" style="1" customWidth="1"/>
-    <col min="10" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
+    <col min="8" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1">
@@ -1507,8 +1508,6 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
     </row>
     <row r="2" ht="21" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1522,8 +1521,6 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
     </row>
     <row r="3" ht="21" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1537,8 +1534,6 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
     </row>
     <row r="4" ht="21" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1552,8 +1547,6 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
     </row>
     <row r="5" ht="21" customHeight="1">
       <c r="A5" t="s" s="2">
@@ -1567,8 +1560,6 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
     </row>
     <row r="6" ht="21" customHeight="1">
       <c r="A6" t="s" s="2">
@@ -1582,8 +1573,6 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
     </row>
     <row r="7" ht="21" customHeight="1">
       <c r="A7" s="8"/>
@@ -1593,8 +1582,6 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
     </row>
     <row r="8" ht="21" customHeight="1">
       <c r="A8" s="8"/>
@@ -1604,8 +1591,6 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
     </row>
     <row r="9" ht="20.65" customHeight="1">
       <c r="A9" s="9"/>
@@ -1615,8 +1600,6 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="A10" s="11"/>
@@ -1626,8 +1609,6 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
       <c r="A11" s="11"/>
@@ -1637,8 +1618,6 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" s="11"/>
@@ -1648,8 +1627,6 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" s="11"/>
@@ -1659,8 +1636,6 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" s="11"/>
@@ -1670,8 +1645,6 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
       <c r="A15" s="11"/>
@@ -1681,8 +1654,6 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="A16" s="11"/>
@@ -1692,74 +1663,6 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>